<commit_message>
Updated flyer and PC list
</commit_message>
<xml_diff>
--- a/2020/sbst-org.xlsx
+++ b/2020/sbst-org.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erik\AppData\Local\Packages\CanonicalGroupLimited.UbuntuonWindows_79rhkp1fndgsc\LocalState\rootfs\home\erik\sbst20\searchbasedsoftwaretesting.github.io\2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A449D729-D453-450A-927E-8CBB3744082B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B388362-9B8F-4D03-889D-F8C42435681F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="9102" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PC" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="69">
   <si>
     <t>PC Member</t>
   </si>
@@ -595,7 +595,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -678,6 +678,9 @@
       <c r="B7" t="s">
         <v>39</v>
       </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
@@ -704,6 +707,9 @@
       </c>
       <c r="B10" s="2" t="s">
         <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">

</xml_diff>